<commit_message>
Updated 19 test cases with loop loading details method
</commit_message>
<xml_diff>
--- a/Test Data/TC_53550_Verify_DC_Unit_For_Multiple_Built_In_Non_Built_In_Isolator_Devices_Integral_Non_Integral_LED_of_PFI.xlsx
+++ b/Test Data/TC_53550_Verify_DC_Unit_For_Multiple_Built_In_Non_Built_In_Isolator_Devices_Integral_Non_Integral_LED_of_PFI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhakaa\Documents\NG Consys Project\Testing\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB237A-224A-426D-8EF5-8E0150F98640}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769BF380-E688-48A7-BC10-4C27CC1E3EBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Device</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>NGC-1139/TC-53550</t>
+  </si>
+  <si>
+    <t>DC Unit Loading Details Name</t>
+  </si>
+  <si>
+    <t>Current (DC Units)</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,6 +545,9 @@
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -552,6 +561,9 @@
         <v>7</v>
       </c>
       <c r="D2" s="13"/>
+      <c r="F2" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">

</xml_diff>